<commit_message>
feat: 更新 excel 模板
</commit_message>
<xml_diff>
--- a/src/templates/template.xlsx
+++ b/src/templates/template.xlsx
@@ -37,7 +37,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>ip</t>
+    <t>host</t>
   </si>
   <si>
     <t>username</t>
@@ -1301,7 +1301,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="6"/>

</xml_diff>